<commit_message>
Renamed custom validator class, provided JSON validation and utf8 sensitive json and XLS
</commit_message>
<xml_diff>
--- a/app/tests/data/xls/tabular.xlsx
+++ b/app/tests/data/xls/tabular.xlsx
@@ -35,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>eenheden</t>
+    <t>hondertallen</t>
   </si>
   <si>
-    <t>tientallen</t>
+    <t>eenheden kolom</t>
   </si>
   <si>
-    <t>hondertallen</t>
+    <t>tientallén kolom</t>
   </si>
 </sst>
 </file>
@@ -387,25 +387,25 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>